<commit_message>
[200~ specified, nothing added.
</commit_message>
<xml_diff>
--- a/Thesis/Product.xlsx
+++ b/Thesis/Product.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Количество по полю Количество</t>
   </si>
@@ -121,78 +121,6 @@
   </si>
   <si>
     <t>Минск</t>
-  </si>
-  <si>
-    <t>БОТИНКИ С БРОГИРОВАНИЕМ НА МАССИВНОЙ ПОДОШВЕ ТЕМНО-КОРИЧНЕВЫЕ 1009-02</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>ДЕРБИ КЛАССИЧЕСКИЕ ТЕМНО-КОРИЧНЕВЫЕ 6805-878</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>БОТИНКИ ВЫСОКИЕ ЧЕРНЫЕ КОЖА 2123-01</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>БОТИНКИ НА ТОЛСТОЙ СПЛОШНОЙ ПОДОШВЕ ТЕМНО-КОРИЧНЕВЫЕ 9075</t>
-  </si>
-  <si>
-    <t>Могилев</t>
-  </si>
-  <si>
-    <t>Туфли женские 1111111</t>
-  </si>
-  <si>
-    <t>Гомель</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>Годно</t>
-  </si>
-  <si>
-    <t>Туфли женские 2222222</t>
-  </si>
-  <si>
-    <t>Витебск</t>
-  </si>
-  <si>
-    <t>Брест</t>
-  </si>
-  <si>
-    <t>Туфли женские 4444444</t>
-  </si>
-  <si>
-    <t>Жлобин</t>
-  </si>
-  <si>
-    <t>Полоцк</t>
-  </si>
-  <si>
-    <t>Туфли женские 8888888</t>
-  </si>
-  <si>
-    <t>Название 4444455</t>
-  </si>
-  <si>
-    <t>Тапочки домашние 2251199</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Тапочки домашние 2261199</t>
-  </si>
-  <si>
-    <t>Тапочки домашние 2271199</t>
   </si>
 </sst>
 </file>
@@ -4463,7 +4391,7 @@
             <xdr:cNvPr id="6" name="Месяц">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8749eb97-e6a0-4447-882d-9c1d7b8a40af}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4467fcd8-d953-4638-a790-57f770be3921}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4483,7 +4411,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="{8749eb97-e6a0-4447-882d-9c1d7b8a40af}"/>
+            <xdr:cNvPr id="6" name="{4467fcd8-d953-4638-a790-57f770be3921}"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -4530,7 +4458,7 @@
             <xdr:cNvPr id="7" name="Год">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2a41f85e-ae24-4990-8b5b-17b7d3d12ce5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{dc94c3f3-2232-41b9-91ed-8019f78efe13}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4550,7 +4478,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="{2a41f85e-ae24-4990-8b5b-17b7d3d12ce5}"/>
+            <xdr:cNvPr id="7" name="{dc94c3f3-2232-41b9-91ed-8019f78efe13}"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -4597,7 +4525,7 @@
             <xdr:cNvPr id="8" name="Продукт">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{b2b1db75-e409-4cb1-a0a0-7cb2c5892b03}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{864a1d8f-879c-4d53-b702-918ed25833c7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4617,7 +4545,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="{b2b1db75-e409-4cb1-a0a0-7cb2c5892b03}"/>
+            <xdr:cNvPr id="8" name="{864a1d8f-879c-4d53-b702-918ed25833c7}"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -4664,7 +4592,7 @@
             <xdr:cNvPr id="9" name="Регион">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ebafb385-8a44-4492-8c81-79282bddf6a2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ead53f97-3ebb-47fa-9047-9f1dfdcdd266}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4684,7 +4612,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="{ebafb385-8a44-4492-8c81-79282bddf6a2}"/>
+            <xdr:cNvPr id="9" name="{ead53f97-3ebb-47fa-9047-9f1dfdcdd266}"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -4757,18 +4685,6 @@
     <cacheField name="Продукт" numFmtId="0">
       <sharedItems containsBlank="1">
         <s v="БОТИНКИ ВЫСОКИЕ НА БАЙКЕ ЧЕРНЫЕ 6538-01"/>
-        <s v="БОТИНКИ С БРОГИРОВАНИЕМ НА МАССИВНОЙ ПОДОШВЕ ТЕМНО-КОРИЧНЕВЫЕ 1009-02"/>
-        <s v="ДЕРБИ КЛАССИЧЕСКИЕ ТЕМНО-КОРИЧНЕВЫЕ 6805-878"/>
-        <s v="БОТИНКИ ВЫСОКИЕ ЧЕРНЫЕ КОЖА 2123-01"/>
-        <s v="БОТИНКИ НА ТОЛСТОЙ СПЛОШНОЙ ПОДОШВЕ ТЕМНО-КОРИЧНЕВЫЕ 9075"/>
-        <s v="Туфли женские 1111111"/>
-        <s v="Туфли женские 2222222"/>
-        <s v="Туфли женские 4444444"/>
-        <s v="Туфли женские 8888888"/>
-        <s v="Название 4444455"/>
-        <s v="Тапочки домашние 2251199"/>
-        <s v="Тапочки домашние 2261199"/>
-        <s v="Тапочки домашние 2271199"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -4778,13 +4694,6 @@
     <cacheField name="Регион" numFmtId="0">
       <sharedItems containsBlank="1">
         <s v="Минск"/>
-        <s v="Могилев"/>
-        <s v="Гомель"/>
-        <s v="Годно"/>
-        <s v="Витебск"/>
-        <s v="Брест"/>
-        <s v="Жлобин"/>
-        <s v="Полоцк"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -4820,36 +4729,17 @@
   <pivotFields count="7">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="15">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="10">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -4894,36 +4784,17 @@
   <pivotFields count="7">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item x="13"/>
+      <items count="3">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="10">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -4987,36 +4858,17 @@
   <pivotFields count="7">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item x="13"/>
+      <items count="3">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="10">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5091,36 +4943,17 @@
   <pivotFields count="7">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item x="13"/>
+      <items count="3">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="10">
-        <item x="8"/>
+      <items count="3">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5195,36 +5028,17 @@
   <pivotFields count="7">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="15">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="10">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5283,7 +5097,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Месяц" xr10:uid="{cfe9b12c-abb1-41ab-9dea-5bb8296f9926}" name="Slicer_Месяц" mc:Ignorable="x xr10">
+<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Месяц" xr10:uid="{a46296e1-e9dc-4ec6-900c-4ee53789e68c}" name="Slicer_Месяц" mc:Ignorable="x xr10">
   <pivotTables>
     <pivotTable name="Сводная таблица1" tabId="7"/>
     <pivotTable name="Сводная таблица2" tabId="3"/>
@@ -5301,7 +5115,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Год" xr10:uid="{e14d3b60-b70d-42c8-a4db-c5ca5367128b}" name="Slicer_Год" mc:Ignorable="x xr10">
+<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Год" xr10:uid="{2da273a2-d5b0-4ac2-adf0-ab01ede39def}" name="Slicer_Год" mc:Ignorable="x xr10">
   <pivotTables>
     <pivotTable name="Сводная таблица1" tabId="7"/>
     <pivotTable name="Сводная таблица2" tabId="3"/>
@@ -5319,7 +5133,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Продукт" xr10:uid="{2c37c0fa-111d-43a8-83b6-4a5457ce7d2d}" name="Slicer_Продукт" mc:Ignorable="x xr10">
+<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Продукт" xr10:uid="{f4b7bb8d-82bd-48c9-80a9-a7f1d876a0b3}" name="Slicer_Продукт" mc:Ignorable="x xr10">
   <pivotTables>
     <pivotTable name="Сводная таблица1" tabId="7"/>
     <pivotTable name="Сводная таблица3" tabId="4"/>
@@ -5328,21 +5142,9 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="6">
-      <items count="14">
+      <items count="2">
         <i x="0" s="1"/>
         <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="3" s="1"/>
-        <i x="4" s="1"/>
-        <i x="5" s="1"/>
-        <i x="6" s="1"/>
-        <i x="7" s="1"/>
-        <i x="8" s="1"/>
-        <i x="9" s="1"/>
-        <i x="10" s="1"/>
-        <i x="11" s="1"/>
-        <i x="12" s="1"/>
-        <i x="13" s="1"/>
       </items>
     </tabular>
   </data>
@@ -5350,7 +5152,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Регион" xr10:uid="{9d2592a0-6d76-4915-8690-5150f0af94f9}" name="Slicer_Регион" mc:Ignorable="x xr10">
+<slicerCacheDefinition xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" sourceName="Регион" xr10:uid="{c57d6044-9dbd-4b35-a0e8-1efe8d544b46}" name="Slicer_Регион" mc:Ignorable="x xr10">
   <pivotTables>
     <pivotTable name="Сводная таблица1" tabId="7"/>
     <pivotTable name="Сводная таблица2" tabId="3"/>
@@ -5359,16 +5161,9 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="6">
-      <items count="9">
+      <items count="2">
         <i x="0" s="1"/>
         <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="3" s="1"/>
-        <i x="4" s="1"/>
-        <i x="5" s="1"/>
-        <i x="6" s="1"/>
-        <i x="7" s="1"/>
-        <i x="8" s="1"/>
       </items>
     </tabular>
   </data>
@@ -5846,7 +5641,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1" style="10"/>
-    <col min="2" max="2" width="83.0880911690848" customWidth="1" style="10"/>
+    <col min="2" max="2" width="45.0300641741071" customWidth="1" style="10"/>
     <col min="3" max="3" width="10.3913982936314" customWidth="1" style="10"/>
     <col min="4" max="4" width="10.0558329990932" customWidth="1" style="10"/>
     <col min="5" max="5" width="14.2442626953125" customWidth="1" style="10"/>
@@ -5901,21 +5696,6 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
-        <v>44752</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="10">
-        <v>5000</v>
-      </c>
       <c r="F4" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -5924,21 +5704,6 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10">
-        <v>44752</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="10">
-        <v>5030</v>
-      </c>
       <c r="F5" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -5947,21 +5712,6 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10">
-        <v>44752</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1040</v>
-      </c>
       <c r="F6" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -5970,21 +5720,6 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10">
-        <v>44752</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="10">
-        <v>9050</v>
-      </c>
       <c r="F7" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -5993,21 +5728,6 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10">
-        <v>44752</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="10">
-        <v>9060</v>
-      </c>
       <c r="F8" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6016,21 +5736,6 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10">
-        <v>44824</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="10">
-        <v>120</v>
-      </c>
       <c r="F9" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6039,21 +5744,6 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10">
-        <v>44665</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="10">
-        <v>100</v>
-      </c>
       <c r="F10" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6062,21 +5752,6 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10">
-        <v>44665</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="10">
-        <v>200</v>
-      </c>
       <c r="F11" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6085,21 +5760,6 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10">
-        <v>44667</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="10">
-        <v>200</v>
-      </c>
       <c r="F12" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6108,21 +5768,6 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10">
-        <v>44667</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="10">
-        <v>200</v>
-      </c>
       <c r="F13" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6131,21 +5776,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10">
-        <v>44669</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="10">
-        <v>100</v>
-      </c>
       <c r="F14" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6154,21 +5784,6 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10">
-        <v>44671</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="10">
-        <v>100</v>
-      </c>
       <c r="F15" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6177,21 +5792,6 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10">
-        <v>44701</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="10">
-        <v>100</v>
-      </c>
       <c r="F16" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6200,21 +5800,6 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10">
-        <v>44723</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="10">
-        <v>300</v>
-      </c>
       <c r="F17" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6223,21 +5808,6 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10">
-        <v>44727</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="10">
-        <v>200</v>
-      </c>
       <c r="F18" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6246,21 +5816,6 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10">
-        <v>44730</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="10">
-        <v>200</v>
-      </c>
       <c r="F19" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6269,21 +5824,6 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10">
-        <v>44750</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="10">
-        <v>250</v>
-      </c>
       <c r="F20" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6292,21 +5832,6 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10">
-        <v>44760</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="10">
-        <v>500</v>
-      </c>
       <c r="F21" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6315,21 +5840,6 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10">
-        <v>44874</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="10">
-        <v>400</v>
-      </c>
       <c r="F22" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6338,21 +5848,6 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="10">
-        <v>44875</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="10">
-        <v>700</v>
-      </c>
       <c r="F23" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6361,21 +5856,6 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="10">
-        <v>44910</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="10">
-        <v>900</v>
-      </c>
       <c r="F24" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6384,21 +5864,6 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10">
-        <v>44910</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="10">
-        <v>800</v>
-      </c>
       <c r="F25" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6407,21 +5872,6 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10">
-        <v>44609</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="10">
-        <v>500</v>
-      </c>
       <c r="F26" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6430,21 +5880,6 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10">
-        <v>44613</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="10">
-        <v>120</v>
-      </c>
       <c r="F27" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6453,21 +5888,6 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10">
-        <v>44613</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="10">
-        <v>230</v>
-      </c>
       <c r="F28" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6476,21 +5896,6 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10">
-        <v>44613</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="10">
-        <v>430</v>
-      </c>
       <c r="F29" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6499,21 +5904,6 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="10">
-        <v>540</v>
-      </c>
       <c r="F30" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6522,21 +5912,6 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="10">
-        <v>750</v>
-      </c>
       <c r="F31" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6545,21 +5920,6 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="10">
-        <v>860</v>
-      </c>
       <c r="F32" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6568,21 +5928,6 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="10">
-        <v>480</v>
-      </c>
       <c r="F33" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6591,21 +5936,6 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="10">
-        <v>690</v>
-      </c>
       <c r="F34" s="10" t="str">
         <f t="shared" si="0"/>
       </c>
@@ -6614,21 +5944,6 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="10">
-        <v>750</v>
-      </c>
       <c r="F35" s="10" t="str">
         <f ref="F35:F66" t="shared" si="2">IF(ISBLANK(A35),"",TEXT(A35,"ММММ"))</f>
       </c>
@@ -6637,21 +5952,6 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="10">
-        <v>590</v>
-      </c>
       <c r="F36" s="10" t="str">
         <f t="shared" si="2"/>
       </c>
@@ -6660,21 +5960,6 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="10">
-        <v>44617</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="10">
-        <v>450</v>
-      </c>
       <c r="F37" s="10" t="str">
         <f t="shared" si="2"/>
       </c>

</xml_diff>